<commit_message>
story 1 en begin story 2
</commit_message>
<xml_diff>
--- a/Kassa/src/bestanden/artikel.xlsx
+++ b/Kassa/src/bestanden/artikel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibre\OneDrive\Documenten\OOO\26_Jacobs_Vandenplas_Vryghem_Kassa_OOO2019\Kassa\src\bestanden\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A7D7B43-8807-4949-91B0-1EC9286EC306}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="19875" windowHeight="7725"/>
+    <workbookView xWindow="2205" yWindow="2295" windowWidth="14250" windowHeight="10275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="artikel" sheetId="1" r:id="rId1"/>
@@ -79,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,13 +617,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -655,9 +669,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -689,9 +703,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -723,9 +755,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -898,20 +948,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="3" max="3" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -928,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -945,7 +995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -962,7 +1012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -979,7 +1029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -996,7 +1046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1013,7 +1063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1030,7 +1080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -1047,7 +1097,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -1064,7 +1114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>10</v>
       </c>

</xml_diff>